<commit_message>
Modification to the dataset
</commit_message>
<xml_diff>
--- a/dataset/Daily sales/ds_excel/2023/Dailysales_05_2023.xlsx
+++ b/dataset/Daily sales/ds_excel/2023/Dailysales_05_2023.xlsx
@@ -924,16 +924,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C26" t="n">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
@@ -943,16 +943,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2537</v>
+        <v>2549</v>
       </c>
       <c r="C27" t="n">
-        <v>8353</v>
+        <v>8401</v>
       </c>
       <c r="D27" t="n">
         <v>15</v>
       </c>
       <c r="E27" t="n">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -966,7 +966,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E204"/>
+  <dimension ref="A1:E202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1934,45 +1934,45 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>272025647628</v>
+        <v>272025627236</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D51" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E51" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>272025627236</v>
+        <v>272025647560</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="D52" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E52" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>272025647560</v>
+        <v>272026258341</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1980,18 +1980,18 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="D53" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E53" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>272026258341</v>
+        <v>272026265845</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1999,18 +1999,18 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>560</v>
+        <v>583</v>
       </c>
       <c r="D54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E54" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>272026265845</v>
+        <v>272025677921</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2018,18 +2018,18 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="D55" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E55" t="n">
-        <v>77.78</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>272025677921</v>
+        <v>272025609101</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2037,18 +2037,18 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>589</v>
+        <v>602</v>
       </c>
       <c r="D56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" t="n">
-        <v>22.22</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>272025609101</v>
+        <v>272025609110</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -2056,56 +2056,56 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>602</v>
+        <v>620</v>
       </c>
       <c r="D57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E57" t="n">
-        <v>33.33</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>272025609110</v>
+        <v>272025609053</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D58" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E58" t="n">
-        <v>88.89</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>272025609053</v>
+        <v>272025627662</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>621</v>
+        <v>633</v>
       </c>
       <c r="D59" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E59" t="n">
-        <v>33.33</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>272025627662</v>
+        <v>272025627231</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -2113,7 +2113,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="D60" t="n">
         <v>5</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>272025627231</v>
+        <v>272025647642</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -2132,10 +2132,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>635</v>
+        <v>662</v>
       </c>
       <c r="D61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E61" t="n">
         <v>88.89</v>
@@ -2143,75 +2143,75 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>272025647642</v>
+        <v>272025647367</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="D62" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E62" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>272025647367</v>
+        <v>272025647383</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>665</v>
+        <v>726</v>
       </c>
       <c r="D63" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>272025647383</v>
+        <v>272025637837</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>726</v>
+        <v>746</v>
       </c>
       <c r="D64" t="n">
         <v>4</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>272025637837</v>
+        <v>272025627692</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>746</v>
+        <v>759</v>
       </c>
       <c r="D65" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E65" t="n">
         <v>22.22</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>272025627692</v>
+        <v>272025627683</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2227,18 +2227,18 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>759</v>
+        <v>767</v>
       </c>
       <c r="D66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E66" t="n">
-        <v>22.22</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>272025627683</v>
+        <v>272025647401</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2246,18 +2246,18 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>767</v>
+        <v>771</v>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E67" t="n">
-        <v>88.89</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>272025647401</v>
+        <v>272025853083</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2265,18 +2265,18 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="D68" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E68" t="n">
-        <v>11.11</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>272025853083</v>
+        <v>272025677714</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -2284,67 +2284,67 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>773</v>
+        <v>779</v>
       </c>
       <c r="D69" t="n">
         <v>4</v>
       </c>
       <c r="E69" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>272025677714</v>
+        <v>272025647446</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>779</v>
+        <v>799</v>
       </c>
       <c r="D70" t="n">
         <v>4</v>
       </c>
       <c r="E70" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>272025627660</v>
+        <v>272025647467</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>782</v>
+        <v>838</v>
       </c>
       <c r="D71" t="n">
         <v>4</v>
       </c>
       <c r="E71" t="n">
-        <v>66.67</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>272025647446</v>
+        <v>272025661631</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>799</v>
+        <v>843</v>
       </c>
       <c r="D72" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
@@ -2352,26 +2352,26 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>272025647467</v>
+        <v>272025627221</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>838</v>
+        <v>845</v>
       </c>
       <c r="D73" t="n">
         <v>4</v>
       </c>
       <c r="E73" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>272025661631</v>
+        <v>272025630867</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2379,18 +2379,18 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>843</v>
+        <v>853</v>
       </c>
       <c r="D74" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>272025627221</v>
+        <v>272025635009</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2398,18 +2398,18 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>845</v>
+        <v>858</v>
       </c>
       <c r="D75" t="n">
         <v>4</v>
       </c>
       <c r="E75" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>272025630867</v>
+        <v>272025647398</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -2417,18 +2417,18 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>853</v>
+        <v>879</v>
       </c>
       <c r="D76" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E76" t="n">
-        <v>88.89</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>272025635009</v>
+        <v>272025647403</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -2436,18 +2436,18 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>858</v>
+        <v>882</v>
       </c>
       <c r="D77" t="n">
         <v>4</v>
       </c>
       <c r="E77" t="n">
-        <v>77.78</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>272025647398</v>
+        <v>272025609125</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -2455,18 +2455,18 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>879</v>
+        <v>888</v>
       </c>
       <c r="D78" t="n">
         <v>5</v>
       </c>
       <c r="E78" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>272025647403</v>
+        <v>272025627885</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -2474,18 +2474,18 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>882</v>
+        <v>893</v>
       </c>
       <c r="D79" t="n">
         <v>4</v>
       </c>
       <c r="E79" t="n">
-        <v>44.44</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>272025609125</v>
+        <v>272025661702</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -2493,18 +2493,18 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>888</v>
+        <v>896</v>
       </c>
       <c r="D80" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E80" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>272025627885</v>
+        <v>272025627731</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -2512,10 +2512,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>893</v>
+        <v>900</v>
       </c>
       <c r="D81" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E81" t="n">
         <v>88.89</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>272025661702</v>
+        <v>272025661716</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -2531,18 +2531,18 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>896</v>
+        <v>903</v>
       </c>
       <c r="D82" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>22.22</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>272025627731</v>
+        <v>272025647445</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -2550,18 +2550,18 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>900</v>
+        <v>928</v>
       </c>
       <c r="D83" t="n">
         <v>5</v>
       </c>
       <c r="E83" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>272025661716</v>
+        <v>272025627458</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -2569,18 +2569,18 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>903</v>
+        <v>939</v>
       </c>
       <c r="D84" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E84" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>272025647445</v>
+        <v>272025660512</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -2588,18 +2588,18 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>928</v>
+        <v>955</v>
       </c>
       <c r="D85" t="n">
         <v>5</v>
       </c>
       <c r="E85" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>272025627458</v>
+        <v>272025647443</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -2607,18 +2607,18 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>939</v>
+        <v>960</v>
       </c>
       <c r="D86" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E86" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>272025660512</v>
+        <v>272025647453</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>955</v>
+        <v>970</v>
       </c>
       <c r="D87" t="n">
         <v>5</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>272025647443</v>
+        <v>272025627180</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -2645,18 +2645,18 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>960</v>
+        <v>978</v>
       </c>
       <c r="D88" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E88" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>272025647453</v>
+        <v>272025647463</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -2664,10 +2664,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>970</v>
+        <v>984</v>
       </c>
       <c r="D89" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E89" t="n">
         <v>88.89</v>
@@ -2675,18 +2675,18 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>272025627180</v>
+        <v>272025647407</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>978</v>
+        <v>1005</v>
       </c>
       <c r="D90" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E90" t="n">
         <v>77.78</v>
@@ -2694,7 +2694,7 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>272025647463</v>
+        <v>272025627256</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -2702,10 +2702,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>984</v>
+        <v>1018</v>
       </c>
       <c r="D91" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E91" t="n">
         <v>88.89</v>
@@ -2713,18 +2713,18 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>272025647407</v>
+        <v>272025647381</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1005</v>
+        <v>1028</v>
       </c>
       <c r="D92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E92" t="n">
         <v>77.78</v>
@@ -2732,26 +2732,26 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>272025627256</v>
+        <v>272025647484</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1018</v>
+        <v>1039</v>
       </c>
       <c r="D93" t="n">
         <v>1</v>
       </c>
       <c r="E93" t="n">
-        <v>88.89</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>272025647381</v>
+        <v>272025647488</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -2759,37 +2759,37 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1028</v>
+        <v>1042</v>
       </c>
       <c r="D94" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E94" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>272025647484</v>
+        <v>272025647497</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1039</v>
+        <v>1045</v>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E95" t="n">
-        <v>33.33</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>272025647488</v>
+        <v>272025647491</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -2797,7 +2797,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1042</v>
+        <v>1050</v>
       </c>
       <c r="D96" t="n">
         <v>4</v>
@@ -2808,7 +2808,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>272025647497</v>
+        <v>272025647475</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -2816,18 +2816,18 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1045</v>
+        <v>1081</v>
       </c>
       <c r="D97" t="n">
         <v>5</v>
       </c>
       <c r="E97" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>272025647491</v>
+        <v>272025609111</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -2835,10 +2835,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1050</v>
+        <v>1085</v>
       </c>
       <c r="D98" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E98" t="n">
         <v>88.89</v>
@@ -2846,26 +2846,26 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>272025647475</v>
+        <v>272025647425</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1081</v>
+        <v>1110</v>
       </c>
       <c r="D99" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E99" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>272025609111</v>
+        <v>272025627182</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -2873,37 +2873,37 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1085</v>
+        <v>1115</v>
       </c>
       <c r="D100" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E100" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>272025647425</v>
+        <v>272025627640</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1110</v>
+        <v>1120</v>
       </c>
       <c r="D101" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E101" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>272025627182</v>
+        <v>272025647436</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -2911,10 +2911,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1115</v>
+        <v>1121</v>
       </c>
       <c r="D102" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E102" t="n">
         <v>66.67</v>
@@ -2922,26 +2922,26 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>272025627640</v>
+        <v>272025637517</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1120</v>
+        <v>1124</v>
       </c>
       <c r="D103" t="n">
         <v>4</v>
       </c>
       <c r="E103" t="n">
-        <v>33.33</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>272025647436</v>
+        <v>272025627226</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -2949,37 +2949,37 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>1121</v>
+        <v>1125</v>
       </c>
       <c r="D104" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E104" t="n">
-        <v>66.67</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>272025637517</v>
+        <v>272025647486</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>1124</v>
+        <v>1127</v>
       </c>
       <c r="D105" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E105" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>272025627226</v>
+        <v>272025627262</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -2987,18 +2987,18 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1125</v>
+        <v>1128</v>
       </c>
       <c r="D106" t="n">
         <v>3</v>
       </c>
       <c r="E106" t="n">
-        <v>11.11</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>272025647486</v>
+        <v>272025627387</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -3006,10 +3006,10 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1127</v>
+        <v>1133</v>
       </c>
       <c r="D107" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E107" t="n">
         <v>88.89</v>
@@ -3017,18 +3017,18 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>272025627262</v>
+        <v>272025647505</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1128</v>
+        <v>1137</v>
       </c>
       <c r="D108" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E108" t="n">
         <v>77.78</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>272025627387</v>
+        <v>272025627594</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -3044,29 +3044,29 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1133</v>
+        <v>1138</v>
       </c>
       <c r="D109" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E109" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>272025647505</v>
+        <v>272025677739</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="D110" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E110" t="n">
         <v>77.78</v>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>272025627594</v>
+        <v>272025647511</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -3082,18 +3082,18 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1138</v>
+        <v>1148</v>
       </c>
       <c r="D111" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E111" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>272025677739</v>
+        <v>272025647510</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -3101,18 +3101,18 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1139</v>
+        <v>1155</v>
       </c>
       <c r="D112" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E112" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>272025647511</v>
+        <v>272025647356</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -3120,18 +3120,18 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1148</v>
+        <v>1164</v>
       </c>
       <c r="D113" t="n">
         <v>4</v>
       </c>
       <c r="E113" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>272025647510</v>
+        <v>272025627192</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -3139,18 +3139,18 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1155</v>
+        <v>1167</v>
       </c>
       <c r="D114" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E114" t="n">
-        <v>88.89</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>272025647356</v>
+        <v>272025647499</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -3158,18 +3158,18 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1164</v>
+        <v>1170</v>
       </c>
       <c r="D115" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E115" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>272025627192</v>
+        <v>272025627254</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -3177,18 +3177,18 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1167</v>
+        <v>1180</v>
       </c>
       <c r="D116" t="n">
         <v>5</v>
       </c>
       <c r="E116" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>272025647499</v>
+        <v>272025647457</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -3196,18 +3196,18 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1170</v>
+        <v>1190</v>
       </c>
       <c r="D117" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E117" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>272025627254</v>
+        <v>272026334041</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -3215,18 +3215,18 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1180</v>
+        <v>1191</v>
       </c>
       <c r="D118" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E118" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>272025647457</v>
+        <v>272025627677</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -3234,37 +3234,37 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1190</v>
+        <v>1199</v>
       </c>
       <c r="D119" t="n">
         <v>4</v>
       </c>
       <c r="E119" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>272026334041</v>
+        <v>272025609122</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1191</v>
+        <v>1203</v>
       </c>
       <c r="D120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E120" t="n">
-        <v>22.22</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>272025627677</v>
+        <v>272025637501</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -3272,37 +3272,37 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1199</v>
+        <v>1211</v>
       </c>
       <c r="D121" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E121" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>272025609122</v>
+        <v>272025627599</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1203</v>
+        <v>1219</v>
       </c>
       <c r="D122" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E122" t="n">
-        <v>11.11</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>272025637501</v>
+        <v>272025616740</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -3310,18 +3310,18 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1211</v>
+        <v>1231</v>
       </c>
       <c r="D123" t="n">
         <v>3</v>
       </c>
       <c r="E123" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>272025627599</v>
+        <v>272026334061</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -3329,37 +3329,37 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1219</v>
+        <v>1233</v>
       </c>
       <c r="D124" t="n">
         <v>4</v>
       </c>
       <c r="E124" t="n">
-        <v>77.78</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>272025616740</v>
+        <v>272025647540</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1231</v>
+        <v>1239</v>
       </c>
       <c r="D125" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E125" t="n">
-        <v>88.89</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>272026334061</v>
+        <v>272025647543</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -3367,56 +3367,56 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1233</v>
+        <v>1242</v>
       </c>
       <c r="D126" t="n">
         <v>4</v>
       </c>
       <c r="E126" t="n">
-        <v>22.22</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>272025647540</v>
+        <v>272025660283</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1239</v>
+        <v>1254</v>
       </c>
       <c r="D127" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E127" t="n">
-        <v>33.33</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>272025647543</v>
+        <v>272025647502</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1242</v>
+        <v>1272</v>
       </c>
       <c r="D128" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E128" t="n">
-        <v>11.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>272025660283</v>
+        <v>272025677684</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -3424,37 +3424,37 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1254</v>
+        <v>1281</v>
       </c>
       <c r="D129" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E129" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>272025647502</v>
+        <v>272025625560</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1272</v>
+        <v>1289</v>
       </c>
       <c r="D130" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E130" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>272025677684</v>
+        <v>272025647529</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -3462,18 +3462,18 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1281</v>
+        <v>1294</v>
       </c>
       <c r="D131" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E131" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>272025625560</v>
+        <v>272025627232</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -3481,18 +3481,18 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1289</v>
+        <v>1325</v>
       </c>
       <c r="D132" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E132" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>272025647529</v>
+        <v>272026330414</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -3500,18 +3500,18 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>1294</v>
+        <v>1334</v>
       </c>
       <c r="D133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E133" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>272025627232</v>
+        <v>272025647376</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -3519,10 +3519,10 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1325</v>
+        <v>1336</v>
       </c>
       <c r="D134" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E134" t="n">
         <v>0</v>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>272026330414</v>
+        <v>272025627450</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -3538,10 +3538,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1334</v>
+        <v>1339</v>
       </c>
       <c r="D135" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E135" t="n">
         <v>88.89</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>272025647376</v>
+        <v>272025647365</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -3557,37 +3557,37 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1336</v>
+        <v>1348</v>
       </c>
       <c r="D136" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E136" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>272025627450</v>
+        <v>272025663156</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>1339</v>
+        <v>1358</v>
       </c>
       <c r="D137" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E137" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>272025647365</v>
+        <v>272025609104</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -3595,37 +3595,37 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1348</v>
+        <v>1377</v>
       </c>
       <c r="D138" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E138" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>272025663156</v>
+        <v>272025664676</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C139" t="n">
-        <v>1358</v>
+        <v>1384</v>
       </c>
       <c r="D139" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E139" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>272025609104</v>
+        <v>272025664932</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -3633,7 +3633,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>1377</v>
+        <v>1389</v>
       </c>
       <c r="D140" t="n">
         <v>5</v>
@@ -3644,7 +3644,7 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>272025664676</v>
+        <v>272025664392</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -3652,10 +3652,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>1384</v>
+        <v>1394</v>
       </c>
       <c r="D141" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E141" t="n">
         <v>88.89</v>
@@ -3663,7 +3663,7 @@
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>272025664932</v>
+        <v>272025663153</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -3671,10 +3671,10 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1389</v>
+        <v>1395</v>
       </c>
       <c r="D142" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E142" t="n">
         <v>77.78</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>272025664392</v>
+        <v>272025627902</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -3690,10 +3690,10 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1394</v>
+        <v>1418</v>
       </c>
       <c r="D143" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E143" t="n">
         <v>88.89</v>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>272025663153</v>
+        <v>272025668632</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -3709,18 +3709,18 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>1395</v>
+        <v>1420</v>
       </c>
       <c r="D144" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E144" t="n">
-        <v>77.78</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>272025627902</v>
+        <v>272026334073</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -3728,18 +3728,18 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>1418</v>
+        <v>1423</v>
       </c>
       <c r="D145" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E145" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>272025668632</v>
+        <v>272025675558</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -3747,37 +3747,37 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1420</v>
+        <v>1428</v>
       </c>
       <c r="D146" t="n">
         <v>3</v>
       </c>
       <c r="E146" t="n">
-        <v>55.56</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>272026334073</v>
+        <v>272026330405</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1423</v>
+        <v>1430</v>
       </c>
       <c r="D147" t="n">
         <v>4</v>
       </c>
       <c r="E147" t="n">
-        <v>0</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>272025675558</v>
+        <v>272025647409</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -3785,37 +3785,37 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1428</v>
+        <v>1433</v>
       </c>
       <c r="D148" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E148" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>272026330405</v>
+        <v>272026326078</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1430</v>
+        <v>1458</v>
       </c>
       <c r="D149" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E149" t="n">
-        <v>11.11</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>272025647409</v>
+        <v>272025627234</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -3823,10 +3823,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>1433</v>
+        <v>0</v>
       </c>
       <c r="D150" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E150" t="n">
         <v>66.67</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>272026326078</v>
+        <v>272025635012</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -3842,10 +3842,10 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>1458</v>
+        <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E151" t="n">
         <v>88.89</v>
@@ -3853,7 +3853,7 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>272025627234</v>
+        <v>272025641528</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -3864,15 +3864,15 @@
         <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E152" t="n">
-        <v>66.67</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>272025635012</v>
+        <v>272025666676</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -3883,15 +3883,15 @@
         <v>0</v>
       </c>
       <c r="D153" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E153" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>272025641528</v>
+        <v>272025677690</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -3902,15 +3902,15 @@
         <v>0</v>
       </c>
       <c r="D154" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E154" t="n">
-        <v>44.44</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>272025666676</v>
+        <v>272025845825</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -3921,15 +3921,15 @@
         <v>0</v>
       </c>
       <c r="D155" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E155" t="n">
-        <v>0</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>272025677690</v>
+        <v>272026769336</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -3940,15 +3940,15 @@
         <v>0</v>
       </c>
       <c r="D156" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E156" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>272025845825</v>
+        <v>272026771781</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -3959,15 +3959,15 @@
         <v>0</v>
       </c>
       <c r="D157" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E157" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>272026769336</v>
+        <v>272027236279</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -3978,15 +3978,15 @@
         <v>0</v>
       </c>
       <c r="D158" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E158" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>272026771781</v>
+        <v>272027301807</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -4000,31 +4000,31 @@
         <v>3</v>
       </c>
       <c r="E159" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>272027236279</v>
+        <v>272027336447</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C160" t="n">
         <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E160" t="n">
-        <v>77.78</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>272027301807</v>
+        <v>272027443002</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -4035,19 +4035,19 @@
         <v>0</v>
       </c>
       <c r="D161" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E161" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>272027336447</v>
+        <v>272027592893</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -4057,12 +4057,12 @@
         <v>4</v>
       </c>
       <c r="E162" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>272027443002</v>
+        <v>272027615470</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -4073,26 +4073,26 @@
         <v>0</v>
       </c>
       <c r="D163" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E163" t="n">
-        <v>33.33</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>272027592893</v>
+        <v>272027646981</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C164" t="n">
         <v>0</v>
       </c>
       <c r="D164" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E164" t="n">
         <v>0</v>
@@ -4100,26 +4100,26 @@
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>272027615470</v>
+        <v>272027764205</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C165" t="n">
         <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E165" t="n">
-        <v>11.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>272027646981</v>
+        <v>272028072828</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -4138,26 +4138,26 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>272027764205</v>
+        <v>272028558309</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C167" t="n">
         <v>0</v>
       </c>
       <c r="D167" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E167" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>272028072828</v>
+        <v>272028559137</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="D168" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E168" t="n">
         <v>0</v>
@@ -4176,45 +4176,45 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>272028558309</v>
+        <v>272028561707</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C169" t="n">
         <v>0</v>
       </c>
       <c r="D169" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E169" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>272028559137</v>
+        <v>272028562938</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C170" t="n">
         <v>0</v>
       </c>
       <c r="D170" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E170" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>272028561707</v>
+        <v>272028605249</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -4225,7 +4225,7 @@
         <v>0</v>
       </c>
       <c r="D171" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E171" t="n">
         <v>0</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>272028562938</v>
+        <v>272028610872</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -4244,19 +4244,19 @@
         <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E172" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>272028605249</v>
+        <v>272028725616</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -4266,69 +4266,69 @@
         <v>2</v>
       </c>
       <c r="E173" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>272028610872</v>
+        <v>272028873224</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C174" t="n">
         <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E174" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>272028725616</v>
+        <v>272029115693</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C175" t="n">
         <v>0</v>
       </c>
       <c r="D175" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E175" t="n">
-        <v>44.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>272028873224</v>
+        <v>272029229165</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C176" t="n">
         <v>0</v>
       </c>
       <c r="D176" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E176" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>272029115693</v>
+        <v>272029282241</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -4339,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="D177" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E177" t="n">
         <v>0</v>
@@ -4347,26 +4347,26 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>272029229165</v>
+        <v>272029286320</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C178" t="n">
         <v>0</v>
       </c>
       <c r="D178" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E178" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>272029282241</v>
+        <v>272029554204</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
@@ -4377,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="D179" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E179" t="n">
         <v>0</v>
@@ -4385,7 +4385,7 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>272029286320</v>
+        <v>272029669154</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
@@ -4404,11 +4404,11 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>272029554204</v>
+        <v>272029728832</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -4423,37 +4423,37 @@
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>272029669154</v>
+        <v>272029743798</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C182" t="n">
         <v>0</v>
       </c>
       <c r="D182" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E182" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>272029728832</v>
+        <v>272029812199</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C183" t="n">
         <v>0</v>
       </c>
       <c r="D183" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E183" t="n">
         <v>0</v>
@@ -4461,7 +4461,7 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>272029743798</v>
+        <v>272029897120</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
@@ -4472,15 +4472,15 @@
         <v>0</v>
       </c>
       <c r="D184" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E184" t="n">
-        <v>44.44</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>272029812199</v>
+        <v>272030043358</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
@@ -4491,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="D185" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E185" t="n">
         <v>0</v>
@@ -4499,26 +4499,26 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>272029897120</v>
+        <v>272030065396</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C186" t="n">
         <v>0</v>
       </c>
       <c r="D186" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E186" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>272030043358</v>
+        <v>272030065415</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
@@ -4529,7 +4529,7 @@
         <v>0</v>
       </c>
       <c r="D187" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E187" t="n">
         <v>0</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>272030065396</v>
+        <v>272030138861</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
@@ -4548,7 +4548,7 @@
         <v>0</v>
       </c>
       <c r="D188" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E188" t="n">
         <v>0</v>
@@ -4556,18 +4556,18 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>272030065415</v>
+        <v>272030166458</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C189" t="n">
         <v>0</v>
       </c>
       <c r="D189" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E189" t="n">
         <v>0</v>
@@ -4575,26 +4575,26 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>272030138861</v>
+        <v>272030201518</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C190" t="n">
         <v>0</v>
       </c>
       <c r="D190" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E190" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>272030166458</v>
+        <v>272030201549</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
@@ -4605,15 +4605,15 @@
         <v>0</v>
       </c>
       <c r="D191" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E191" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>272030201518</v>
+        <v>272030201552</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
@@ -4627,12 +4627,12 @@
         <v>4</v>
       </c>
       <c r="E192" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>272030201549</v>
+        <v>272030201560</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
@@ -4643,19 +4643,19 @@
         <v>0</v>
       </c>
       <c r="D193" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E193" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>272030201552</v>
+        <v>272030211548</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -4670,7 +4670,7 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>272030201560</v>
+        <v>272030211550</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
@@ -4689,18 +4689,18 @@
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>272030211548</v>
+        <v>272030211551</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C196" t="n">
         <v>0</v>
       </c>
       <c r="D196" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E196" t="n">
         <v>0</v>
@@ -4708,18 +4708,18 @@
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>272030211550</v>
+        <v>272030211553</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C197" t="n">
         <v>0</v>
       </c>
       <c r="D197" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E197" t="n">
         <v>0</v>
@@ -4727,18 +4727,18 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>272030211551</v>
+        <v>272030211555</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C198" t="n">
         <v>0</v>
       </c>
       <c r="D198" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E198" t="n">
         <v>0</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>272030211553</v>
+        <v>272030211556</v>
       </c>
       <c r="B199" t="inlineStr">
         <is>
@@ -4757,7 +4757,7 @@
         <v>0</v>
       </c>
       <c r="D199" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E199" t="n">
         <v>0</v>
@@ -4765,18 +4765,18 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>272030211555</v>
+        <v>272030211558</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C200" t="n">
         <v>0</v>
       </c>
       <c r="D200" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E200" t="n">
         <v>0</v>
@@ -4784,7 +4784,7 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>272030211556</v>
+        <v>272030211561</v>
       </c>
       <c r="B201" t="inlineStr">
         <is>
@@ -4803,58 +4803,20 @@
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>272030211558</v>
+        <v>272030211563</v>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C202" t="n">
         <v>0</v>
       </c>
       <c r="D202" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E202" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="n">
-        <v>272030211561</v>
-      </c>
-      <c r="B203" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C203" t="n">
-        <v>0</v>
-      </c>
-      <c r="D203" t="n">
-        <v>3</v>
-      </c>
-      <c r="E203" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="n">
-        <v>272030211563</v>
-      </c>
-      <c r="B204" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C204" t="n">
-        <v>0</v>
-      </c>
-      <c r="D204" t="n">
-        <v>3</v>
-      </c>
-      <c r="E204" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding colours to percentage column
</commit_message>
<xml_diff>
--- a/dataset/Daily sales/ds_excel/2023/Dailysales_05_2023.xlsx
+++ b/dataset/Daily sales/ds_excel/2023/Dailysales_05_2023.xlsx
@@ -924,16 +924,16 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C26" t="n">
-        <v>124</v>
+        <v>279</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27">
@@ -943,16 +943,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2549</v>
+        <v>2594</v>
       </c>
       <c r="C27" t="n">
-        <v>8401</v>
+        <v>8556</v>
       </c>
       <c r="D27" t="n">
         <v>15</v>
       </c>
       <c r="E27" t="n">
-        <v>494</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -966,7 +966,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E192"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>272025662605</v>
+        <v>272025627203</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1581,10 +1581,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="D32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32" t="n">
         <v>88.89</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>272025627203</v>
+        <v>272025677653</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1600,18 +1600,18 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="D33" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E33" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>272025677653</v>
+        <v>272025627193</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1619,18 +1619,18 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="D34" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E34" t="n">
-        <v>66.67</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>272025627193</v>
+        <v>272025647609</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1638,18 +1638,18 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>384</v>
+        <v>401</v>
       </c>
       <c r="D35" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E35" t="n">
-        <v>55.56</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>272025647609</v>
+        <v>272025661043</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1657,18 +1657,18 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>401</v>
+        <v>426</v>
       </c>
       <c r="D36" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E36" t="n">
-        <v>77.78</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>272025661043</v>
+        <v>272025609060</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1676,18 +1676,18 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D37" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E37" t="n">
-        <v>44.44</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>272025609060</v>
+        <v>272025647612</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1695,18 +1695,18 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="D38" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E38" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>272025647612</v>
+        <v>272025647509</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1714,10 +1714,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>428</v>
+        <v>451</v>
       </c>
       <c r="D39" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E39" t="n">
         <v>77.78</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>272025647509</v>
+        <v>272025627243</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1733,18 +1733,18 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E40" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>272025627243</v>
+        <v>272025647542</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1752,18 +1752,18 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>453</v>
+        <v>474</v>
       </c>
       <c r="D41" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>272025647542</v>
+        <v>272025627289</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1771,18 +1771,18 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="D42" t="n">
         <v>5</v>
       </c>
       <c r="E42" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>272025627289</v>
+        <v>272025662330</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1790,18 +1790,18 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="D43" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E43" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>272025662330</v>
+        <v>272025627185</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1809,56 +1809,56 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>484</v>
+        <v>496</v>
       </c>
       <c r="D44" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>272025627185</v>
+        <v>272025678593</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>496</v>
+        <v>510</v>
       </c>
       <c r="D45" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E45" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>272025678593</v>
+        <v>272025627620</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D46" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E46" t="n">
-        <v>77.78</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>272025627620</v>
+        <v>272025609109</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1866,18 +1866,18 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D47" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E47" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>272025609109</v>
+        <v>272025664561</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1885,18 +1885,18 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="D48" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E48" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>272025664561</v>
+        <v>272025627831</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1904,10 +1904,10 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="D49" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49" t="n">
         <v>88.89</v>
@@ -1915,45 +1915,45 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>272025627831</v>
+        <v>272025627236</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>525</v>
+        <v>547</v>
       </c>
       <c r="D50" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E50" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>272025627236</v>
+        <v>272025647560</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>547</v>
+        <v>553</v>
       </c>
       <c r="D51" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E51" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>272025647560</v>
+        <v>272026258341</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1961,18 +1961,18 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="D52" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E52" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>272026258341</v>
+        <v>272026265845</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1980,18 +1980,18 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>560</v>
+        <v>583</v>
       </c>
       <c r="D53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E53" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>272026265845</v>
+        <v>272025677921</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1999,18 +1999,18 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="D54" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E54" t="n">
-        <v>77.78</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>272025677921</v>
+        <v>272025609101</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2018,18 +2018,18 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>589</v>
+        <v>602</v>
       </c>
       <c r="D55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E55" t="n">
-        <v>22.22</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>272025609101</v>
+        <v>272025609110</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2037,56 +2037,56 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>602</v>
+        <v>620</v>
       </c>
       <c r="D56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E56" t="n">
-        <v>33.33</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>272025609110</v>
+        <v>272025609053</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D57" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E57" t="n">
-        <v>88.89</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>272025609053</v>
+        <v>272025627662</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>621</v>
+        <v>633</v>
       </c>
       <c r="D58" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E58" t="n">
-        <v>33.33</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>272025627662</v>
+        <v>272025627231</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2094,7 +2094,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="D59" t="n">
         <v>5</v>
@@ -2105,7 +2105,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>272025627231</v>
+        <v>272025647642</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -2113,10 +2113,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>635</v>
+        <v>662</v>
       </c>
       <c r="D60" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E60" t="n">
         <v>88.89</v>
@@ -2124,75 +2124,75 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>272025647642</v>
+        <v>272025647367</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="D61" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E61" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>272025647367</v>
+        <v>272025647383</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>665</v>
+        <v>726</v>
       </c>
       <c r="D62" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E62" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>272025647383</v>
+        <v>272025637837</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>726</v>
+        <v>746</v>
       </c>
       <c r="D63" t="n">
         <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>272025637837</v>
+        <v>272025627692</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>746</v>
+        <v>759</v>
       </c>
       <c r="D64" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E64" t="n">
         <v>22.22</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>272025627692</v>
+        <v>272025627683</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2208,18 +2208,18 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>759</v>
+        <v>767</v>
       </c>
       <c r="D65" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E65" t="n">
-        <v>22.22</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>272025627683</v>
+        <v>272025647401</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2227,18 +2227,18 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>767</v>
+        <v>771</v>
       </c>
       <c r="D66" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E66" t="n">
-        <v>88.89</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>272025647401</v>
+        <v>272025853083</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2246,18 +2246,18 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="D67" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E67" t="n">
-        <v>11.11</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>272025853083</v>
+        <v>272025677714</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2265,37 +2265,37 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>773</v>
+        <v>779</v>
       </c>
       <c r="D68" t="n">
         <v>4</v>
       </c>
       <c r="E68" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>272025677714</v>
+        <v>272025647446</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>779</v>
+        <v>799</v>
       </c>
       <c r="D69" t="n">
         <v>4</v>
       </c>
       <c r="E69" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>272025647446</v>
+        <v>272025647467</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -2303,37 +2303,37 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>799</v>
+        <v>838</v>
       </c>
       <c r="D70" t="n">
         <v>4</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>272025647467</v>
+        <v>272025661631</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>838</v>
+        <v>843</v>
       </c>
       <c r="D71" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E71" t="n">
-        <v>55.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>272025661631</v>
+        <v>272025627221</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -2341,18 +2341,18 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="D72" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>272025627221</v>
+        <v>272025630867</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -2360,10 +2360,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>845</v>
+        <v>853</v>
       </c>
       <c r="D73" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E73" t="n">
         <v>88.89</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>272025630867</v>
+        <v>272025635009</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2379,18 +2379,18 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>853</v>
+        <v>858</v>
       </c>
       <c r="D74" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E74" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>272025635009</v>
+        <v>272025647398</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2398,18 +2398,18 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>858</v>
+        <v>879</v>
       </c>
       <c r="D75" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E75" t="n">
-        <v>77.78</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>272025647398</v>
+        <v>272025647403</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -2417,18 +2417,18 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="D76" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E76" t="n">
-        <v>55.56</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>272025647403</v>
+        <v>272025609125</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -2436,18 +2436,18 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>882</v>
+        <v>888</v>
       </c>
       <c r="D77" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E77" t="n">
-        <v>44.44</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>272025609125</v>
+        <v>272025627885</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -2455,10 +2455,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>888</v>
+        <v>893</v>
       </c>
       <c r="D78" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E78" t="n">
         <v>88.89</v>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>272025627885</v>
+        <v>272025661702</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -2474,18 +2474,18 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="D79" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E79" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>272025661702</v>
+        <v>272025627731</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -2493,18 +2493,18 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>896</v>
+        <v>900</v>
       </c>
       <c r="D80" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E80" t="n">
-        <v>22.22</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>272025627731</v>
+        <v>272025647445</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -2512,18 +2512,18 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>900</v>
+        <v>928</v>
       </c>
       <c r="D81" t="n">
         <v>5</v>
       </c>
       <c r="E81" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>272025661716</v>
+        <v>272025627458</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -2531,18 +2531,18 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>903</v>
+        <v>939</v>
       </c>
       <c r="D82" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E82" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>272025647445</v>
+        <v>272025660512</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -2550,18 +2550,18 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>928</v>
+        <v>955</v>
       </c>
       <c r="D83" t="n">
         <v>5</v>
       </c>
       <c r="E83" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>272025627458</v>
+        <v>272025647443</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -2569,18 +2569,18 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>939</v>
+        <v>960</v>
       </c>
       <c r="D84" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E84" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>272025660512</v>
+        <v>272025647453</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -2588,7 +2588,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>955</v>
+        <v>970</v>
       </c>
       <c r="D85" t="n">
         <v>5</v>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>272025647443</v>
+        <v>272025627180</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -2607,18 +2607,18 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>960</v>
+        <v>978</v>
       </c>
       <c r="D86" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E86" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>272025647453</v>
+        <v>272025647463</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -2626,10 +2626,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>970</v>
+        <v>984</v>
       </c>
       <c r="D87" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E87" t="n">
         <v>88.89</v>
@@ -2637,18 +2637,18 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>272025627180</v>
+        <v>272025647407</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>978</v>
+        <v>1005</v>
       </c>
       <c r="D88" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E88" t="n">
         <v>77.78</v>
@@ -2656,7 +2656,7 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>272025647463</v>
+        <v>272025627256</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -2664,10 +2664,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>984</v>
+        <v>1018</v>
       </c>
       <c r="D89" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E89" t="n">
         <v>88.89</v>
@@ -2675,18 +2675,18 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>272025647407</v>
+        <v>272025647381</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1005</v>
+        <v>1028</v>
       </c>
       <c r="D90" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E90" t="n">
         <v>77.78</v>
@@ -2694,26 +2694,26 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>272025627256</v>
+        <v>272025647484</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1018</v>
+        <v>1039</v>
       </c>
       <c r="D91" t="n">
         <v>1</v>
       </c>
       <c r="E91" t="n">
-        <v>88.89</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>272025647381</v>
+        <v>272025647488</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -2721,37 +2721,37 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1028</v>
+        <v>1042</v>
       </c>
       <c r="D92" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E92" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>272025647484</v>
+        <v>272025647497</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1039</v>
+        <v>1045</v>
       </c>
       <c r="D93" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E93" t="n">
-        <v>33.33</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>272025647488</v>
+        <v>272025647491</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -2759,7 +2759,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1042</v>
+        <v>1050</v>
       </c>
       <c r="D94" t="n">
         <v>4</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>272025647497</v>
+        <v>272025647475</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -2778,18 +2778,18 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1045</v>
+        <v>1081</v>
       </c>
       <c r="D95" t="n">
         <v>5</v>
       </c>
       <c r="E95" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>272025647491</v>
+        <v>272025609111</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -2797,10 +2797,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1050</v>
+        <v>1085</v>
       </c>
       <c r="D96" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E96" t="n">
         <v>88.89</v>
@@ -2808,26 +2808,26 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>272025647475</v>
+        <v>272025647425</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1081</v>
+        <v>1110</v>
       </c>
       <c r="D97" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E97" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>272025609111</v>
+        <v>272025627182</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -2835,37 +2835,37 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1085</v>
+        <v>1115</v>
       </c>
       <c r="D98" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E98" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>272025647425</v>
+        <v>272025627640</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1110</v>
+        <v>1120</v>
       </c>
       <c r="D99" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E99" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>272025627182</v>
+        <v>272025647436</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -2873,10 +2873,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1115</v>
+        <v>1121</v>
       </c>
       <c r="D100" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E100" t="n">
         <v>66.67</v>
@@ -2884,26 +2884,26 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>272025627640</v>
+        <v>272025637517</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1120</v>
+        <v>1124</v>
       </c>
       <c r="D101" t="n">
         <v>4</v>
       </c>
       <c r="E101" t="n">
-        <v>33.33</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>272025647436</v>
+        <v>272025627226</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -2911,37 +2911,37 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1121</v>
+        <v>1125</v>
       </c>
       <c r="D102" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E102" t="n">
-        <v>66.67</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>272025637517</v>
+        <v>272025647486</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1124</v>
+        <v>1127</v>
       </c>
       <c r="D103" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E103" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>272025627226</v>
+        <v>272025627262</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -2949,18 +2949,18 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>1125</v>
+        <v>1128</v>
       </c>
       <c r="D104" t="n">
         <v>3</v>
       </c>
       <c r="E104" t="n">
-        <v>11.11</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>272025647486</v>
+        <v>272025627387</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -2968,10 +2968,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>1127</v>
+        <v>1133</v>
       </c>
       <c r="D105" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E105" t="n">
         <v>88.89</v>
@@ -2979,18 +2979,18 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>272025627262</v>
+        <v>272025647505</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1128</v>
+        <v>1137</v>
       </c>
       <c r="D106" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E106" t="n">
         <v>77.78</v>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>272025627387</v>
+        <v>272025627594</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -3006,29 +3006,29 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1133</v>
+        <v>1138</v>
       </c>
       <c r="D107" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E107" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>272025647505</v>
+        <v>272025677739</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="D108" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E108" t="n">
         <v>77.78</v>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>272025627594</v>
+        <v>272025647511</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -3044,18 +3044,18 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1138</v>
+        <v>1148</v>
       </c>
       <c r="D109" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E109" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>272025677739</v>
+        <v>272025647510</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -3063,18 +3063,18 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1139</v>
+        <v>1155</v>
       </c>
       <c r="D110" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E110" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>272025647511</v>
+        <v>272025647356</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -3082,18 +3082,18 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1148</v>
+        <v>1164</v>
       </c>
       <c r="D111" t="n">
         <v>4</v>
       </c>
       <c r="E111" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>272025647510</v>
+        <v>272025627192</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -3101,18 +3101,18 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1155</v>
+        <v>1167</v>
       </c>
       <c r="D112" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E112" t="n">
-        <v>88.89</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>272025647356</v>
+        <v>272025627254</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -3120,10 +3120,10 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1164</v>
+        <v>1180</v>
       </c>
       <c r="D113" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E113" t="n">
         <v>88.89</v>
@@ -3131,7 +3131,7 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>272025627192</v>
+        <v>272025647457</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -3139,18 +3139,18 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1167</v>
+        <v>1190</v>
       </c>
       <c r="D114" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E114" t="n">
-        <v>55.56</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>272025647499</v>
+        <v>272026334041</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -3158,18 +3158,18 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1170</v>
+        <v>1191</v>
       </c>
       <c r="D115" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E115" t="n">
-        <v>77.78</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>272025627254</v>
+        <v>272025627677</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -3177,37 +3177,37 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1180</v>
+        <v>1199</v>
       </c>
       <c r="D116" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E116" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>272025647457</v>
+        <v>272025609122</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1190</v>
+        <v>1203</v>
       </c>
       <c r="D117" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E117" t="n">
-        <v>66.67</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>272026334041</v>
+        <v>272025637501</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -3215,18 +3215,18 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1191</v>
+        <v>1211</v>
       </c>
       <c r="D118" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E118" t="n">
-        <v>22.22</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>272025627677</v>
+        <v>272025627599</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -3234,7 +3234,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1199</v>
+        <v>1219</v>
       </c>
       <c r="D119" t="n">
         <v>4</v>
@@ -3245,26 +3245,26 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>272025609122</v>
+        <v>272025616740</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1203</v>
+        <v>1231</v>
       </c>
       <c r="D120" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E120" t="n">
-        <v>11.11</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>272025637501</v>
+        <v>272026334061</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -3272,37 +3272,37 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1211</v>
+        <v>1233</v>
       </c>
       <c r="D121" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E121" t="n">
-        <v>66.67</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>272025627599</v>
+        <v>272025647540</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1219</v>
+        <v>1239</v>
       </c>
       <c r="D122" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E122" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>272025616740</v>
+        <v>272025647543</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -3310,18 +3310,18 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1231</v>
+        <v>1242</v>
       </c>
       <c r="D123" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E123" t="n">
-        <v>88.89</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>272026334061</v>
+        <v>272025660283</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -3329,18 +3329,18 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1233</v>
+        <v>1254</v>
       </c>
       <c r="D124" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E124" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>272025647540</v>
+        <v>272025647502</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -3348,18 +3348,18 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1239</v>
+        <v>1272</v>
       </c>
       <c r="D125" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E125" t="n">
-        <v>33.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>272025647543</v>
+        <v>272025677684</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -3367,18 +3367,18 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1242</v>
+        <v>1281</v>
       </c>
       <c r="D126" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E126" t="n">
-        <v>11.11</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>272025660283</v>
+        <v>272025625560</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -3386,29 +3386,29 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1254</v>
+        <v>1289</v>
       </c>
       <c r="D127" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E127" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>272025647502</v>
+        <v>272025627232</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1272</v>
+        <v>1325</v>
       </c>
       <c r="D128" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E128" t="n">
         <v>0</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>272025677684</v>
+        <v>272026330414</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -3424,10 +3424,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1281</v>
+        <v>1334</v>
       </c>
       <c r="D129" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E129" t="n">
         <v>88.89</v>
@@ -3435,7 +3435,7 @@
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>272025625560</v>
+        <v>272025647376</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -3443,18 +3443,18 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1289</v>
+        <v>1336</v>
       </c>
       <c r="D130" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E130" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>272025647529</v>
+        <v>272025627450</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -3462,18 +3462,18 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1294</v>
+        <v>1339</v>
       </c>
       <c r="D131" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E131" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>272025627232</v>
+        <v>272025647365</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -3481,37 +3481,37 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1325</v>
+        <v>1348</v>
       </c>
       <c r="D132" t="n">
         <v>4</v>
       </c>
       <c r="E132" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>272026330414</v>
+        <v>272025663156</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>1334</v>
+        <v>1358</v>
       </c>
       <c r="D133" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E133" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>272025647376</v>
+        <v>272025609104</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -3519,18 +3519,18 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1336</v>
+        <v>1377</v>
       </c>
       <c r="D134" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E134" t="n">
-        <v>0</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>272025627450</v>
+        <v>272025664932</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -3538,18 +3538,18 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1339</v>
+        <v>1389</v>
       </c>
       <c r="D135" t="n">
         <v>5</v>
       </c>
       <c r="E135" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>272025647365</v>
+        <v>272025664392</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -3557,10 +3557,10 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1348</v>
+        <v>1394</v>
       </c>
       <c r="D136" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E136" t="n">
         <v>88.89</v>
@@ -3568,26 +3568,26 @@
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>272025663156</v>
+        <v>272025663153</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>1358</v>
+        <v>1395</v>
       </c>
       <c r="D137" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E137" t="n">
-        <v>0</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>272025609104</v>
+        <v>272025627902</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -3595,18 +3595,18 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1377</v>
+        <v>1418</v>
       </c>
       <c r="D138" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E138" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>272025664676</v>
+        <v>272025668632</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -3614,18 +3614,18 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>1384</v>
+        <v>1420</v>
       </c>
       <c r="D139" t="n">
         <v>3</v>
       </c>
       <c r="E139" t="n">
-        <v>88.89</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>272025664932</v>
+        <v>272026334073</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -3633,18 +3633,18 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>1389</v>
+        <v>1423</v>
       </c>
       <c r="D140" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E140" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>272025664392</v>
+        <v>272025675558</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -3652,37 +3652,37 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>1394</v>
+        <v>1428</v>
       </c>
       <c r="D141" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E141" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>272025663153</v>
+        <v>272026330405</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1395</v>
+        <v>1430</v>
       </c>
       <c r="D142" t="n">
         <v>4</v>
       </c>
       <c r="E142" t="n">
-        <v>77.78</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>272025627902</v>
+        <v>272025647409</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -3690,18 +3690,18 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1418</v>
+        <v>1433</v>
       </c>
       <c r="D143" t="n">
         <v>7</v>
       </c>
       <c r="E143" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>272025668632</v>
+        <v>272025627234</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -3709,18 +3709,18 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>1420</v>
+        <v>0</v>
       </c>
       <c r="D144" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E144" t="n">
-        <v>55.56</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>272026334073</v>
+        <v>272025635012</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -3728,18 +3728,18 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>1423</v>
+        <v>0</v>
       </c>
       <c r="D145" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E145" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>272025675558</v>
+        <v>272025641528</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -3747,37 +3747,37 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>1428</v>
+        <v>0</v>
       </c>
       <c r="D146" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E146" t="n">
-        <v>77.78</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>272026330405</v>
+        <v>272025666676</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>1430</v>
+        <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E147" t="n">
-        <v>11.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>272025647409</v>
+        <v>272026769336</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -3785,10 +3785,10 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>1433</v>
+        <v>0</v>
       </c>
       <c r="D148" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E148" t="n">
         <v>66.67</v>
@@ -3796,7 +3796,7 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>272026326078</v>
+        <v>272026771781</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -3804,18 +3804,18 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>1458</v>
+        <v>0</v>
       </c>
       <c r="D149" t="n">
         <v>3</v>
       </c>
       <c r="E149" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>272025627234</v>
+        <v>272027236279</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -3826,15 +3826,15 @@
         <v>0</v>
       </c>
       <c r="D150" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E150" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>272025635012</v>
+        <v>272027301807</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -3845,34 +3845,34 @@
         <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E151" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>272025641528</v>
+        <v>272027336447</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C152" t="n">
         <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E152" t="n">
-        <v>44.44</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>272025666676</v>
+        <v>272027443002</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -3883,15 +3883,15 @@
         <v>0</v>
       </c>
       <c r="D153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E153" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>272025677690</v>
+        <v>272027592893</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -3902,15 +3902,15 @@
         <v>0</v>
       </c>
       <c r="D154" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E154" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>272025845825</v>
+        <v>272027615470</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -3921,57 +3921,57 @@
         <v>0</v>
       </c>
       <c r="D155" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E155" t="n">
-        <v>66.67</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>272026769336</v>
+        <v>272027646981</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C156" t="n">
         <v>0</v>
       </c>
       <c r="D156" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E156" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>272026771781</v>
+        <v>272027764205</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C157" t="n">
         <v>0</v>
       </c>
       <c r="D157" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E157" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>272027236279</v>
+        <v>272028072828</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -3981,23 +3981,23 @@
         <v>3</v>
       </c>
       <c r="E158" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>272027301807</v>
+        <v>272028559137</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C159" t="n">
         <v>0</v>
       </c>
       <c r="D159" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E159" t="n">
         <v>0</v>
@@ -4005,7 +4005,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>272027336447</v>
+        <v>272028561707</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -4016,15 +4016,15 @@
         <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E160" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>272027443002</v>
+        <v>272028562938</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -4035,26 +4035,26 @@
         <v>0</v>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E161" t="n">
-        <v>33.33</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>272027592893</v>
+        <v>272028605249</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C162" t="n">
         <v>0</v>
       </c>
       <c r="D162" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E162" t="n">
         <v>0</v>
@@ -4062,7 +4062,7 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>272027615470</v>
+        <v>272028610872</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -4076,31 +4076,31 @@
         <v>4</v>
       </c>
       <c r="E163" t="n">
-        <v>11.11</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>272027646981</v>
+        <v>272028725616</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C164" t="n">
         <v>0</v>
       </c>
       <c r="D164" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E164" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>272027764205</v>
+        <v>272028873224</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -4111,7 +4111,7 @@
         <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E165" t="n">
         <v>0</v>
@@ -4119,7 +4119,7 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>272028072828</v>
+        <v>272029115693</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -4130,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="D166" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E166" t="n">
         <v>0</v>
@@ -4138,26 +4138,26 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>272028558309</v>
+        <v>272029282241</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C167" t="n">
         <v>0</v>
       </c>
       <c r="D167" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E167" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>272028559137</v>
+        <v>272029286320</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="D168" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E168" t="n">
         <v>0</v>
@@ -4176,7 +4176,7 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>272028561707</v>
+        <v>272029554204</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -4195,11 +4195,11 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>272028562938</v>
+        <v>272029669154</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -4209,23 +4209,23 @@
         <v>2</v>
       </c>
       <c r="E170" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>272028605249</v>
+        <v>272029728832</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C171" t="n">
         <v>0</v>
       </c>
       <c r="D171" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E171" t="n">
         <v>0</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>272028610872</v>
+        <v>272029743798</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -4244,53 +4244,53 @@
         <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E172" t="n">
-        <v>77.78</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>272028725616</v>
+        <v>272029812199</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C173" t="n">
         <v>0</v>
       </c>
       <c r="D173" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E173" t="n">
-        <v>44.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>272028873224</v>
+        <v>272029897120</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C174" t="n">
         <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E174" t="n">
-        <v>0</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>272029115693</v>
+        <v>272030043358</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -4301,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="D175" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E175" t="n">
         <v>0</v>
@@ -4309,26 +4309,26 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>272029229165</v>
+        <v>272030065396</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C176" t="n">
         <v>0</v>
       </c>
       <c r="D176" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E176" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>272029282241</v>
+        <v>272030065415</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -4339,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="D177" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E177" t="n">
         <v>0</v>
@@ -4347,7 +4347,7 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>272029286320</v>
+        <v>272030138861</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -4366,18 +4366,18 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>272029554204</v>
+        <v>272030166458</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C179" t="n">
         <v>0</v>
       </c>
       <c r="D179" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E179" t="n">
         <v>0</v>
@@ -4385,26 +4385,26 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>272029669154</v>
+        <v>272030201518</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C180" t="n">
         <v>0</v>
       </c>
       <c r="D180" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E180" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>272029728832</v>
+        <v>272030201549</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
@@ -4415,15 +4415,15 @@
         <v>0</v>
       </c>
       <c r="D181" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E181" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>272029743798</v>
+        <v>272030201552</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
@@ -4434,19 +4434,19 @@
         <v>0</v>
       </c>
       <c r="D182" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E182" t="n">
-        <v>44.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>272029812199</v>
+        <v>272030201560</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -4461,37 +4461,37 @@
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>272029897120</v>
+        <v>272030211548</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C184" t="n">
         <v>0</v>
       </c>
       <c r="D184" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E184" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>272030043358</v>
+        <v>272030211550</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C185" t="n">
         <v>0</v>
       </c>
       <c r="D185" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E185" t="n">
         <v>0</v>
@@ -4499,11 +4499,11 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>272030065396</v>
+        <v>272030211551</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -4518,7 +4518,7 @@
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>272030065415</v>
+        <v>272030211553</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
@@ -4529,7 +4529,7 @@
         <v>0</v>
       </c>
       <c r="D187" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E187" t="n">
         <v>0</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>272030138861</v>
+        <v>272030211555</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
@@ -4548,7 +4548,7 @@
         <v>0</v>
       </c>
       <c r="D188" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E188" t="n">
         <v>0</v>
@@ -4556,18 +4556,18 @@
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>272030166458</v>
+        <v>272030211556</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C189" t="n">
         <v>0</v>
       </c>
       <c r="D189" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E189" t="n">
         <v>0</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>272030201518</v>
+        <v>272030211558</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
@@ -4586,237 +4586,47 @@
         <v>0</v>
       </c>
       <c r="D190" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E190" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>272030201549</v>
+        <v>272030211561</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C191" t="n">
         <v>0</v>
       </c>
       <c r="D191" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E191" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>272030201552</v>
+        <v>272030211563</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C192" t="n">
         <v>0</v>
       </c>
       <c r="D192" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E192" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="n">
-        <v>272030201560</v>
-      </c>
-      <c r="B193" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C193" t="n">
-        <v>0</v>
-      </c>
-      <c r="D193" t="n">
-        <v>3</v>
-      </c>
-      <c r="E193" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="n">
-        <v>272030211548</v>
-      </c>
-      <c r="B194" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C194" t="n">
-        <v>0</v>
-      </c>
-      <c r="D194" t="n">
-        <v>4</v>
-      </c>
-      <c r="E194" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="n">
-        <v>272030211550</v>
-      </c>
-      <c r="B195" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C195" t="n">
-        <v>0</v>
-      </c>
-      <c r="D195" t="n">
-        <v>3</v>
-      </c>
-      <c r="E195" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="n">
-        <v>272030211551</v>
-      </c>
-      <c r="B196" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C196" t="n">
-        <v>0</v>
-      </c>
-      <c r="D196" t="n">
-        <v>1</v>
-      </c>
-      <c r="E196" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="n">
-        <v>272030211553</v>
-      </c>
-      <c r="B197" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C197" t="n">
-        <v>0</v>
-      </c>
-      <c r="D197" t="n">
-        <v>5</v>
-      </c>
-      <c r="E197" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="n">
-        <v>272030211555</v>
-      </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C198" t="n">
-        <v>0</v>
-      </c>
-      <c r="D198" t="n">
-        <v>3</v>
-      </c>
-      <c r="E198" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="n">
-        <v>272030211556</v>
-      </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C199" t="n">
-        <v>0</v>
-      </c>
-      <c r="D199" t="n">
-        <v>3</v>
-      </c>
-      <c r="E199" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="n">
-        <v>272030211558</v>
-      </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C200" t="n">
-        <v>0</v>
-      </c>
-      <c r="D200" t="n">
-        <v>5</v>
-      </c>
-      <c r="E200" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="n">
-        <v>272030211561</v>
-      </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C201" t="n">
-        <v>0</v>
-      </c>
-      <c r="D201" t="n">
-        <v>3</v>
-      </c>
-      <c r="E201" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="n">
-        <v>272030211563</v>
-      </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C202" t="n">
-        <v>0</v>
-      </c>
-      <c r="D202" t="n">
-        <v>3</v>
-      </c>
-      <c r="E202" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Making UI changes to arrows and headers
</commit_message>
<xml_diff>
--- a/dataset/Daily sales/ds_excel/2023/Dailysales_05_2023.xlsx
+++ b/dataset/Daily sales/ds_excel/2023/Dailysales_05_2023.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -939,20 +939,39 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
+          <t>2023-05-28</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>45</v>
+      </c>
+      <c r="C27" t="n">
+        <v>180</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B27" t="n">
-        <v>2594</v>
-      </c>
-      <c r="C27" t="n">
-        <v>8556</v>
-      </c>
-      <c r="D27" t="n">
+      <c r="B28" t="n">
+        <v>2639</v>
+      </c>
+      <c r="C28" t="n">
+        <v>8736</v>
+      </c>
+      <c r="D28" t="n">
         <v>15</v>
       </c>
-      <c r="E27" t="n">
-        <v>505</v>
+      <c r="E28" t="n">
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -966,7 +985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E192"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -997,7 +1016,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Percentage</t>
+          <t>Probability</t>
         </is>
       </c>
     </row>
@@ -1307,7 +1326,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>272025647687</v>
+        <v>272025609058</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1315,10 +1334,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="D18" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18" t="n">
         <v>88.89</v>
@@ -1326,45 +1345,45 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>272025609058</v>
+        <v>272025647685</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E19" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>272025647685</v>
+        <v>272025609054</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>272025609054</v>
+        <v>272025647541</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1372,48 +1391,48 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>218</v>
+        <v>257</v>
       </c>
       <c r="D21" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E21" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>272025627445</v>
+        <v>272025627179</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>255</v>
+        <v>273</v>
       </c>
       <c r="D22" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" t="n">
-        <v>88.89</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>272025647541</v>
+        <v>272025627346</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>257</v>
+        <v>280</v>
       </c>
       <c r="D23" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
@@ -1421,7 +1440,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>272025627179</v>
+        <v>272025627340</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1429,37 +1448,37 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="D24" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>272025627346</v>
+        <v>272025662865</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="D25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>272025662762</v>
+        <v>272025627357</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1467,10 +1486,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E26" t="n">
         <v>66.67</v>
@@ -1478,7 +1497,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>272025627340</v>
+        <v>272025647591</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1486,10 +1505,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>292</v>
+        <v>340</v>
       </c>
       <c r="D27" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E27" t="n">
         <v>88.89</v>
@@ -1497,7 +1516,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>272025662865</v>
+        <v>272025677679</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1505,18 +1524,18 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>296</v>
+        <v>350</v>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E28" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>272025627357</v>
+        <v>272025627203</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1524,18 +1543,18 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>312</v>
+        <v>360</v>
       </c>
       <c r="D29" t="n">
         <v>4</v>
       </c>
       <c r="E29" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>272025647591</v>
+        <v>272025677653</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1543,18 +1562,18 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>340</v>
+        <v>364</v>
       </c>
       <c r="D30" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E30" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>272025677679</v>
+        <v>272025627193</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1562,18 +1581,18 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>350</v>
+        <v>384</v>
       </c>
       <c r="D31" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E31" t="n">
-        <v>66.67</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>272025627203</v>
+        <v>272025647609</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1581,18 +1600,18 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>360</v>
+        <v>401</v>
       </c>
       <c r="D32" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>272025677653</v>
+        <v>272025661043</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1600,18 +1619,18 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>364</v>
+        <v>426</v>
       </c>
       <c r="D33" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E33" t="n">
-        <v>66.67</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>272025627193</v>
+        <v>272025609060</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1619,18 +1638,18 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>384</v>
+        <v>427</v>
       </c>
       <c r="D34" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E34" t="n">
-        <v>55.56</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>272025647609</v>
+        <v>272025647612</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1638,10 +1657,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>401</v>
+        <v>428</v>
       </c>
       <c r="D35" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E35" t="n">
         <v>77.78</v>
@@ -1649,7 +1668,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>272025661043</v>
+        <v>272025647509</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1657,18 +1676,18 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>426</v>
+        <v>451</v>
       </c>
       <c r="D36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E36" t="n">
-        <v>44.44</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>272025609060</v>
+        <v>272025627243</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1676,18 +1695,18 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>427</v>
+        <v>453</v>
       </c>
       <c r="D37" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E37" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>272025647612</v>
+        <v>272025647542</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1695,18 +1714,18 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>428</v>
+        <v>474</v>
       </c>
       <c r="D38" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E38" t="n">
-        <v>77.78</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>272025647509</v>
+        <v>272025627289</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1714,18 +1733,18 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>451</v>
+        <v>476</v>
       </c>
       <c r="D39" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E39" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>272025627243</v>
+        <v>272025662330</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1733,10 +1752,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>453</v>
+        <v>484</v>
       </c>
       <c r="D40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" t="n">
         <v>0</v>
@@ -1744,7 +1763,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>272025647542</v>
+        <v>272025627185</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1752,37 +1771,37 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>474</v>
+        <v>496</v>
       </c>
       <c r="D41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E41" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>272025627289</v>
+        <v>272025678593</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="D42" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>272025662330</v>
+        <v>272025627620</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1790,18 +1809,18 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>484</v>
+        <v>512</v>
       </c>
       <c r="D43" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>272025627185</v>
+        <v>272025609109</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1809,48 +1828,48 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>496</v>
+        <v>515</v>
       </c>
       <c r="D44" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E44" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>272025678593</v>
+        <v>272025664561</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="D45" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E45" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>272025627620</v>
+        <v>272025627236</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>512</v>
+        <v>547</v>
       </c>
       <c r="D46" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E46" t="n">
         <v>22.22</v>
@@ -1858,7 +1877,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>272025609109</v>
+        <v>272026265845</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1866,10 +1885,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>515</v>
+        <v>583</v>
       </c>
       <c r="D47" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E47" t="n">
         <v>77.78</v>
@@ -1877,7 +1896,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>272025664561</v>
+        <v>272025677921</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1885,18 +1904,18 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>518</v>
+        <v>589</v>
       </c>
       <c r="D48" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E48" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>272025627831</v>
+        <v>272025609101</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1904,56 +1923,56 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>525</v>
+        <v>602</v>
       </c>
       <c r="D49" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E49" t="n">
-        <v>88.89</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>272025627236</v>
+        <v>272025609110</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>547</v>
+        <v>620</v>
       </c>
       <c r="D50" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E50" t="n">
-        <v>22.22</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>272025647560</v>
+        <v>272025609053</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>553</v>
+        <v>621</v>
       </c>
       <c r="D51" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E51" t="n">
-        <v>77.78</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>272026258341</v>
+        <v>272025627231</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1961,7 +1980,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>560</v>
+        <v>635</v>
       </c>
       <c r="D52" t="n">
         <v>5</v>
@@ -1972,7 +1991,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>272026265845</v>
+        <v>272025647642</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1980,29 +1999,29 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>583</v>
+        <v>662</v>
       </c>
       <c r="D53" t="n">
         <v>4</v>
       </c>
       <c r="E53" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>272025677921</v>
+        <v>272025647367</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>589</v>
+        <v>665</v>
       </c>
       <c r="D54" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E54" t="n">
         <v>22.22</v>
@@ -2010,7 +2029,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>272025609101</v>
+        <v>272025647383</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2018,56 +2037,56 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>602</v>
+        <v>726</v>
       </c>
       <c r="D55" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E55" t="n">
-        <v>33.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>272025609110</v>
+        <v>272025637837</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>620</v>
+        <v>746</v>
       </c>
       <c r="D56" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E56" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>272025609053</v>
+        <v>272025627692</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>621</v>
+        <v>759</v>
       </c>
       <c r="D57" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E57" t="n">
-        <v>33.33</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>272025627662</v>
+        <v>272025627683</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -2075,10 +2094,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>633</v>
+        <v>767</v>
       </c>
       <c r="D58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E58" t="n">
         <v>88.89</v>
@@ -2086,7 +2105,7 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>272025627231</v>
+        <v>272025647401</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2094,18 +2113,18 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>635</v>
+        <v>771</v>
       </c>
       <c r="D59" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E59" t="n">
-        <v>88.89</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>272025647642</v>
+        <v>272025853083</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -2113,7 +2132,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>662</v>
+        <v>773</v>
       </c>
       <c r="D60" t="n">
         <v>4</v>
@@ -2124,34 +2143,34 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>272025647367</v>
+        <v>272025677714</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>665</v>
+        <v>779</v>
       </c>
       <c r="D61" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E61" t="n">
-        <v>22.22</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>272025647383</v>
+        <v>272025647446</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>726</v>
+        <v>799</v>
       </c>
       <c r="D62" t="n">
         <v>4</v>
@@ -2162,7 +2181,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>272025637837</v>
+        <v>272025647467</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -2170,18 +2189,18 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>746</v>
+        <v>838</v>
       </c>
       <c r="D63" t="n">
         <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>22.22</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>272025627692</v>
+        <v>272025661631</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -2189,18 +2208,18 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>759</v>
+        <v>843</v>
       </c>
       <c r="D64" t="n">
         <v>5</v>
       </c>
       <c r="E64" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>272025627683</v>
+        <v>272025627221</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2208,7 +2227,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>767</v>
+        <v>845</v>
       </c>
       <c r="D65" t="n">
         <v>4</v>
@@ -2219,7 +2238,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>272025647401</v>
+        <v>272025630867</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2227,18 +2246,18 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>771</v>
+        <v>853</v>
       </c>
       <c r="D66" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E66" t="n">
-        <v>11.11</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>272025853083</v>
+        <v>272025635009</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2246,18 +2265,18 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>773</v>
+        <v>858</v>
       </c>
       <c r="D67" t="n">
         <v>4</v>
       </c>
       <c r="E67" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>272025677714</v>
+        <v>272025647398</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2265,56 +2284,56 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>779</v>
+        <v>879</v>
       </c>
       <c r="D68" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E68" t="n">
-        <v>66.67</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>272025647446</v>
+        <v>272025647403</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>799</v>
+        <v>882</v>
       </c>
       <c r="D69" t="n">
         <v>4</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>272025647467</v>
+        <v>272025609125</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>838</v>
+        <v>888</v>
       </c>
       <c r="D70" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E70" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>272025661631</v>
+        <v>272025627885</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -2322,18 +2341,18 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>843</v>
+        <v>893</v>
       </c>
       <c r="D71" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>272025627221</v>
+        <v>272025661702</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -2341,18 +2360,18 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>845</v>
+        <v>896</v>
       </c>
       <c r="D72" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E72" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>272025630867</v>
+        <v>272025627731</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -2360,10 +2379,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>853</v>
+        <v>900</v>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E73" t="n">
         <v>88.89</v>
@@ -2371,7 +2390,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>272025635009</v>
+        <v>272025647445</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2379,18 +2398,18 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>858</v>
+        <v>928</v>
       </c>
       <c r="D74" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E74" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>272025647398</v>
+        <v>272025627458</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2398,18 +2417,18 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>879</v>
+        <v>939</v>
       </c>
       <c r="D75" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E75" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>272025647403</v>
+        <v>272025660512</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -2417,18 +2436,18 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>882</v>
+        <v>955</v>
       </c>
       <c r="D76" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E76" t="n">
-        <v>44.44</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>272025609125</v>
+        <v>272025647443</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -2436,18 +2455,18 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>888</v>
+        <v>960</v>
       </c>
       <c r="D77" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E77" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>272025627885</v>
+        <v>272025647453</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -2455,10 +2474,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>893</v>
+        <v>970</v>
       </c>
       <c r="D78" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E78" t="n">
         <v>88.89</v>
@@ -2466,7 +2485,7 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>272025661702</v>
+        <v>272025627180</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -2474,18 +2493,18 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>896</v>
+        <v>978</v>
       </c>
       <c r="D79" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E79" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>272025627731</v>
+        <v>272025647463</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -2493,10 +2512,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>900</v>
+        <v>984</v>
       </c>
       <c r="D80" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E80" t="n">
         <v>88.89</v>
@@ -2504,26 +2523,26 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>272025647445</v>
+        <v>272025647407</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>928</v>
+        <v>1005</v>
       </c>
       <c r="D81" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E81" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>272025627458</v>
+        <v>272025627256</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -2531,10 +2550,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>939</v>
+        <v>1018</v>
       </c>
       <c r="D82" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E82" t="n">
         <v>88.89</v>
@@ -2542,7 +2561,7 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>272025660512</v>
+        <v>272025647381</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -2550,37 +2569,37 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>955</v>
+        <v>1028</v>
       </c>
       <c r="D83" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E83" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>272025647443</v>
+        <v>272025647484</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>960</v>
+        <v>1039</v>
       </c>
       <c r="D84" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
-        <v>22.22</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>272025647453</v>
+        <v>272025647488</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -2588,10 +2607,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>970</v>
+        <v>1042</v>
       </c>
       <c r="D85" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E85" t="n">
         <v>88.89</v>
@@ -2599,7 +2618,7 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>272025627180</v>
+        <v>272025647497</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -2607,10 +2626,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>978</v>
+        <v>1045</v>
       </c>
       <c r="D86" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E86" t="n">
         <v>77.78</v>
@@ -2618,7 +2637,7 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>272025647463</v>
+        <v>272025647475</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -2626,10 +2645,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>984</v>
+        <v>1081</v>
       </c>
       <c r="D87" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E87" t="n">
         <v>88.89</v>
@@ -2637,45 +2656,45 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>272025647407</v>
+        <v>272025609111</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1005</v>
+        <v>1085</v>
       </c>
       <c r="D88" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E88" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>272025627256</v>
+        <v>272025647425</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1018</v>
+        <v>1110</v>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E89" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>272025647381</v>
+        <v>272025627182</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -2683,29 +2702,29 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>1028</v>
+        <v>1115</v>
       </c>
       <c r="D90" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E90" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>272025647484</v>
+        <v>272025627640</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1039</v>
+        <v>1120</v>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E91" t="n">
         <v>33.33</v>
@@ -2713,7 +2732,7 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>272025647488</v>
+        <v>272025647436</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -2721,37 +2740,37 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1042</v>
+        <v>1121</v>
       </c>
       <c r="D92" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E92" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>272025647497</v>
+        <v>272025637517</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1045</v>
+        <v>1124</v>
       </c>
       <c r="D93" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E93" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>272025647491</v>
+        <v>272025627226</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -2759,18 +2778,18 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1050</v>
+        <v>1125</v>
       </c>
       <c r="D94" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E94" t="n">
-        <v>88.89</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>272025647475</v>
+        <v>272025647486</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -2778,10 +2797,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1081</v>
+        <v>1127</v>
       </c>
       <c r="D95" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E95" t="n">
         <v>88.89</v>
@@ -2789,7 +2808,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>272025609111</v>
+        <v>272025627262</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -2797,56 +2816,56 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1085</v>
+        <v>1128</v>
       </c>
       <c r="D96" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E96" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>272025647425</v>
+        <v>272025627387</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1110</v>
+        <v>1133</v>
       </c>
       <c r="D97" t="n">
         <v>8</v>
       </c>
       <c r="E97" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>272025627182</v>
+        <v>272025647505</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1115</v>
+        <v>1137</v>
       </c>
       <c r="D98" t="n">
         <v>4</v>
       </c>
       <c r="E98" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>272025627640</v>
+        <v>272025627594</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -2854,18 +2873,18 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1120</v>
+        <v>1138</v>
       </c>
       <c r="D99" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E99" t="n">
-        <v>33.33</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>272025647436</v>
+        <v>272025677739</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -2873,37 +2892,37 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1121</v>
+        <v>1139</v>
       </c>
       <c r="D100" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E100" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>272025637517</v>
+        <v>272025647511</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1124</v>
+        <v>1148</v>
       </c>
       <c r="D101" t="n">
         <v>4</v>
       </c>
       <c r="E101" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>272025627226</v>
+        <v>272025647510</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -2911,18 +2930,18 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1125</v>
+        <v>1155</v>
       </c>
       <c r="D102" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E102" t="n">
-        <v>11.11</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>272025647486</v>
+        <v>272025647356</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -2930,10 +2949,10 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1127</v>
+        <v>1164</v>
       </c>
       <c r="D103" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E103" t="n">
         <v>88.89</v>
@@ -2941,7 +2960,7 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>272025627262</v>
+        <v>272025627192</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -2949,18 +2968,18 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>1128</v>
+        <v>1167</v>
       </c>
       <c r="D104" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E104" t="n">
-        <v>77.78</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>272025627387</v>
+        <v>272025627254</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -2968,10 +2987,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>1133</v>
+        <v>1180</v>
       </c>
       <c r="D105" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E105" t="n">
         <v>88.89</v>
@@ -2979,26 +2998,26 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>272025647505</v>
+        <v>272025647457</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1137</v>
+        <v>1190</v>
       </c>
       <c r="D106" t="n">
         <v>4</v>
       </c>
       <c r="E106" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>272025627594</v>
+        <v>272026334041</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -3006,18 +3025,18 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1138</v>
+        <v>1191</v>
       </c>
       <c r="D107" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E107" t="n">
-        <v>66.67</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>272025677739</v>
+        <v>272025627677</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -3025,10 +3044,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1139</v>
+        <v>1199</v>
       </c>
       <c r="D108" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E108" t="n">
         <v>77.78</v>
@@ -3036,26 +3055,26 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>272025647511</v>
+        <v>272025609122</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1148</v>
+        <v>1203</v>
       </c>
       <c r="D109" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E109" t="n">
-        <v>0</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>272025647510</v>
+        <v>272025637501</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -3063,18 +3082,18 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1155</v>
+        <v>1211</v>
       </c>
       <c r="D110" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E110" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>272025647356</v>
+        <v>272025627599</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -3082,18 +3101,18 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1164</v>
+        <v>1219</v>
       </c>
       <c r="D111" t="n">
         <v>4</v>
       </c>
       <c r="E111" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>272025627192</v>
+        <v>272025616740</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -3101,18 +3120,18 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1167</v>
+        <v>1231</v>
       </c>
       <c r="D112" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E112" t="n">
-        <v>55.56</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>272025627254</v>
+        <v>272026334061</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -3120,37 +3139,37 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1180</v>
+        <v>1233</v>
       </c>
       <c r="D113" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E113" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>272025647457</v>
+        <v>272025647540</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1190</v>
+        <v>1239</v>
       </c>
       <c r="D114" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E114" t="n">
-        <v>66.67</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>272026334041</v>
+        <v>272025647543</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -3158,18 +3177,18 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1191</v>
+        <v>1242</v>
       </c>
       <c r="D115" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E115" t="n">
-        <v>22.22</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>272025627677</v>
+        <v>272025660283</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -3177,10 +3196,10 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1199</v>
+        <v>1254</v>
       </c>
       <c r="D116" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E116" t="n">
         <v>77.78</v>
@@ -3188,7 +3207,7 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>272025609122</v>
+        <v>272025647502</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -3196,18 +3215,18 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1203</v>
+        <v>1272</v>
       </c>
       <c r="D117" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E117" t="n">
-        <v>11.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>272025637501</v>
+        <v>272025677684</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -3215,18 +3234,18 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1211</v>
+        <v>1281</v>
       </c>
       <c r="D118" t="n">
         <v>3</v>
       </c>
       <c r="E118" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>272025627599</v>
+        <v>272025625560</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -3234,18 +3253,18 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1219</v>
+        <v>1289</v>
       </c>
       <c r="D119" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E119" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>272025616740</v>
+        <v>272025627232</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -3253,18 +3272,18 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1231</v>
+        <v>1325</v>
       </c>
       <c r="D120" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E120" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>272026334061</v>
+        <v>272026330414</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -3272,37 +3291,37 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1233</v>
+        <v>1334</v>
       </c>
       <c r="D121" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E121" t="n">
-        <v>22.22</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>272025647540</v>
+        <v>272025647376</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1239</v>
+        <v>1336</v>
       </c>
       <c r="D122" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E122" t="n">
-        <v>33.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>272025647543</v>
+        <v>272025627450</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -3310,18 +3329,18 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1242</v>
+        <v>1339</v>
       </c>
       <c r="D123" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E123" t="n">
-        <v>11.11</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>272025660283</v>
+        <v>272025647365</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -3329,18 +3348,18 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1254</v>
+        <v>1348</v>
       </c>
       <c r="D124" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E124" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>272025647502</v>
+        <v>272025663156</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -3348,10 +3367,10 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1272</v>
+        <v>1358</v>
       </c>
       <c r="D125" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E125" t="n">
         <v>0</v>
@@ -3359,7 +3378,7 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>272025677684</v>
+        <v>272025609104</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -3367,18 +3386,18 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1281</v>
+        <v>1377</v>
       </c>
       <c r="D126" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E126" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>272025625560</v>
+        <v>272025664392</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -3386,10 +3405,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1289</v>
+        <v>1394</v>
       </c>
       <c r="D127" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E127" t="n">
         <v>88.89</v>
@@ -3397,7 +3416,7 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>272025627232</v>
+        <v>272025627902</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -3405,18 +3424,18 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1325</v>
+        <v>1418</v>
       </c>
       <c r="D128" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E128" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>272026330414</v>
+        <v>272025668632</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -3424,18 +3443,18 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1334</v>
+        <v>1420</v>
       </c>
       <c r="D129" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E129" t="n">
-        <v>88.89</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>272025647376</v>
+        <v>272026334073</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -3443,10 +3462,10 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1336</v>
+        <v>1423</v>
       </c>
       <c r="D130" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E130" t="n">
         <v>0</v>
@@ -3454,7 +3473,7 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>272025627450</v>
+        <v>272025675558</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -3462,56 +3481,56 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1339</v>
+        <v>1428</v>
       </c>
       <c r="D131" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E131" t="n">
-        <v>88.89</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>272025647365</v>
+        <v>272026330405</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1348</v>
+        <v>1430</v>
       </c>
       <c r="D132" t="n">
         <v>4</v>
       </c>
       <c r="E132" t="n">
-        <v>88.89</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>272025663156</v>
+        <v>272025647409</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>1358</v>
+        <v>1433</v>
       </c>
       <c r="D133" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E133" t="n">
-        <v>0</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>272025609104</v>
+        <v>272025627234</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -3519,18 +3538,18 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1377</v>
+        <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E134" t="n">
-        <v>77.78</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>272025664932</v>
+        <v>272025635012</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -3538,18 +3557,18 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>1389</v>
+        <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E135" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>272025664392</v>
+        <v>272025641528</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -3557,18 +3576,18 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>1394</v>
+        <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E136" t="n">
-        <v>88.89</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>272025663153</v>
+        <v>272025666676</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -3576,18 +3595,18 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>1395</v>
+        <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E137" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>272025627902</v>
+        <v>272026769336</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -3595,18 +3614,18 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>1418</v>
+        <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E138" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>272025668632</v>
+        <v>272026771781</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -3614,18 +3633,18 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>1420</v>
+        <v>0</v>
       </c>
       <c r="D139" t="n">
         <v>3</v>
       </c>
       <c r="E139" t="n">
-        <v>55.56</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>272026334073</v>
+        <v>272027236279</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -3633,37 +3652,37 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>1423</v>
+        <v>0</v>
       </c>
       <c r="D140" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E140" t="n">
-        <v>0</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>272025675558</v>
+        <v>272027301807</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>1428</v>
+        <v>0</v>
       </c>
       <c r="D141" t="n">
         <v>3</v>
       </c>
       <c r="E141" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>272026330405</v>
+        <v>272027336447</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -3671,18 +3690,18 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>1430</v>
+        <v>0</v>
       </c>
       <c r="D142" t="n">
         <v>4</v>
       </c>
       <c r="E142" t="n">
-        <v>11.11</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>272025647409</v>
+        <v>272027443002</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -3690,18 +3709,18 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>1433</v>
+        <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E143" t="n">
-        <v>66.67</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>272025627234</v>
+        <v>272027592893</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -3712,15 +3731,15 @@
         <v>0</v>
       </c>
       <c r="D144" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E144" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>272025635012</v>
+        <v>272027615470</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -3731,45 +3750,45 @@
         <v>0</v>
       </c>
       <c r="D145" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E145" t="n">
-        <v>88.89</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>272025641528</v>
+        <v>272027646981</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C146" t="n">
         <v>0</v>
       </c>
       <c r="D146" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E146" t="n">
-        <v>44.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>272025666676</v>
+        <v>272027764205</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C147" t="n">
         <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E147" t="n">
         <v>0</v>
@@ -3777,64 +3796,64 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>272026769336</v>
+        <v>272028072828</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C148" t="n">
         <v>0</v>
       </c>
       <c r="D148" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E148" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>272026771781</v>
+        <v>272028559137</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C149" t="n">
         <v>0</v>
       </c>
       <c r="D149" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E149" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>272027236279</v>
+        <v>272028561707</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C150" t="n">
         <v>0</v>
       </c>
       <c r="D150" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E150" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>272027301807</v>
+        <v>272028562938</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -3845,15 +3864,15 @@
         <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E151" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>272027336447</v>
+        <v>272028605249</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -3864,15 +3883,15 @@
         <v>0</v>
       </c>
       <c r="D152" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E152" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>272027443002</v>
+        <v>272028610872</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -3883,15 +3902,15 @@
         <v>0</v>
       </c>
       <c r="D153" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E153" t="n">
-        <v>33.33</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>272027592893</v>
+        <v>272028725616</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -3902,34 +3921,34 @@
         <v>0</v>
       </c>
       <c r="D154" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E154" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>272027615470</v>
+        <v>272028873224</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C155" t="n">
         <v>0</v>
       </c>
       <c r="D155" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E155" t="n">
-        <v>11.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>272027646981</v>
+        <v>272029115693</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -3940,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="D156" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E156" t="n">
         <v>0</v>
@@ -3948,7 +3967,7 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>272027764205</v>
+        <v>272029282241</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -3967,7 +3986,7 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>272028072828</v>
+        <v>272029286320</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -3978,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="D158" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E158" t="n">
         <v>0</v>
@@ -3986,7 +4005,7 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>272028559137</v>
+        <v>272029554204</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -3997,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="D159" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E159" t="n">
         <v>0</v>
@@ -4005,7 +4024,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>272028561707</v>
+        <v>272029669154</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -4016,7 +4035,7 @@
         <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E160" t="n">
         <v>0</v>
@@ -4024,7 +4043,7 @@
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>272028562938</v>
+        <v>272029728832</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -4035,53 +4054,53 @@
         <v>0</v>
       </c>
       <c r="D161" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E161" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>272028605249</v>
+        <v>272029743798</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C162" t="n">
         <v>0</v>
       </c>
       <c r="D162" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E162" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>272028610872</v>
+        <v>272029812199</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C163" t="n">
         <v>0</v>
       </c>
       <c r="D163" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E163" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>272028725616</v>
+        <v>272029897120</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -4092,15 +4111,15 @@
         <v>0</v>
       </c>
       <c r="D164" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E164" t="n">
-        <v>44.44</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>272028873224</v>
+        <v>272030043358</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -4111,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E165" t="n">
         <v>0</v>
@@ -4119,7 +4138,7 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>272029115693</v>
+        <v>272030065396</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -4130,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="D166" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E166" t="n">
         <v>0</v>
@@ -4138,7 +4157,7 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>272029282241</v>
+        <v>272030065415</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -4149,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="D167" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E167" t="n">
         <v>0</v>
@@ -4157,7 +4176,7 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>272029286320</v>
+        <v>272030138861</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -4176,18 +4195,18 @@
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>272029554204</v>
+        <v>272030166458</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C169" t="n">
         <v>0</v>
       </c>
       <c r="D169" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E169" t="n">
         <v>0</v>
@@ -4195,26 +4214,26 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>272029669154</v>
+        <v>272030201549</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C170" t="n">
         <v>0</v>
       </c>
       <c r="D170" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E170" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>272029728832</v>
+        <v>272030201552</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -4225,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="D171" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E171" t="n">
         <v>0</v>
@@ -4233,7 +4252,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>272029743798</v>
+        <v>272030201560</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -4244,15 +4263,15 @@
         <v>0</v>
       </c>
       <c r="D172" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E172" t="n">
-        <v>44.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>272029812199</v>
+        <v>272030211548</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -4263,7 +4282,7 @@
         <v>0</v>
       </c>
       <c r="D173" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E173" t="n">
         <v>0</v>
@@ -4271,7 +4290,7 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>272029897120</v>
+        <v>272030211550</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -4285,16 +4304,16 @@
         <v>3</v>
       </c>
       <c r="E174" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>272030043358</v>
+        <v>272030211551</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -4309,7 +4328,7 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>272030065396</v>
+        <v>272030211553</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -4320,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="D176" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E176" t="n">
         <v>0</v>
@@ -4328,7 +4347,7 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>272030065415</v>
+        <v>272030211555</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
@@ -4339,7 +4358,7 @@
         <v>0</v>
       </c>
       <c r="D177" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E177" t="n">
         <v>0</v>
@@ -4347,7 +4366,7 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>272030138861</v>
+        <v>272030211556</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -4358,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="D178" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E178" t="n">
         <v>0</v>
@@ -4366,7 +4385,7 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>272030166458</v>
+        <v>272030211558</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
@@ -4377,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="D179" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E179" t="n">
         <v>0</v>
@@ -4385,248 +4404,39 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>272030201518</v>
+        <v>272030211561</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C180" t="n">
         <v>0</v>
       </c>
       <c r="D180" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E180" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>272030201549</v>
+        <v>272030211563</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C181" t="n">
         <v>0</v>
       </c>
       <c r="D181" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E181" t="n">
-        <v>22.22</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="n">
-        <v>272030201552</v>
-      </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C182" t="n">
-        <v>0</v>
-      </c>
-      <c r="D182" t="n">
-        <v>4</v>
-      </c>
-      <c r="E182" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="n">
-        <v>272030201560</v>
-      </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C183" t="n">
-        <v>0</v>
-      </c>
-      <c r="D183" t="n">
-        <v>3</v>
-      </c>
-      <c r="E183" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="n">
-        <v>272030211548</v>
-      </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C184" t="n">
-        <v>0</v>
-      </c>
-      <c r="D184" t="n">
-        <v>4</v>
-      </c>
-      <c r="E184" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="n">
-        <v>272030211550</v>
-      </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C185" t="n">
-        <v>0</v>
-      </c>
-      <c r="D185" t="n">
-        <v>3</v>
-      </c>
-      <c r="E185" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="n">
-        <v>272030211551</v>
-      </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C186" t="n">
-        <v>0</v>
-      </c>
-      <c r="D186" t="n">
-        <v>1</v>
-      </c>
-      <c r="E186" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="n">
-        <v>272030211553</v>
-      </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C187" t="n">
-        <v>0</v>
-      </c>
-      <c r="D187" t="n">
-        <v>5</v>
-      </c>
-      <c r="E187" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="n">
-        <v>272030211555</v>
-      </c>
-      <c r="B188" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C188" t="n">
-        <v>0</v>
-      </c>
-      <c r="D188" t="n">
-        <v>3</v>
-      </c>
-      <c r="E188" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="n">
-        <v>272030211556</v>
-      </c>
-      <c r="B189" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C189" t="n">
-        <v>0</v>
-      </c>
-      <c r="D189" t="n">
-        <v>3</v>
-      </c>
-      <c r="E189" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="n">
-        <v>272030211558</v>
-      </c>
-      <c r="B190" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C190" t="n">
-        <v>0</v>
-      </c>
-      <c r="D190" t="n">
-        <v>5</v>
-      </c>
-      <c r="E190" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="n">
-        <v>272030211561</v>
-      </c>
-      <c r="B191" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C191" t="n">
-        <v>0</v>
-      </c>
-      <c r="D191" t="n">
-        <v>3</v>
-      </c>
-      <c r="E191" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="n">
-        <v>272030211563</v>
-      </c>
-      <c r="B192" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C192" t="n">
-        <v>0</v>
-      </c>
-      <c r="D192" t="n">
-        <v>3</v>
-      </c>
-      <c r="E192" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Error handling in last bold line of availability table
</commit_message>
<xml_diff>
--- a/dataset/Daily sales/ds_excel/2023/Dailysales_05_2023.xlsx
+++ b/dataset/Daily sales/ds_excel/2023/Dailysales_05_2023.xlsx
@@ -943,16 +943,16 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C27" t="n">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28">
@@ -962,16 +962,16 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2639</v>
+        <v>2645</v>
       </c>
       <c r="C28" t="n">
-        <v>8736</v>
+        <v>8760</v>
       </c>
       <c r="D28" t="n">
         <v>15</v>
       </c>
       <c r="E28" t="n">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>
@@ -985,7 +985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E181"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>272025627254</v>
+        <v>272025647457</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -2987,18 +2987,18 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>1180</v>
+        <v>1190</v>
       </c>
       <c r="D105" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E105" t="n">
-        <v>88.89</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>272025647457</v>
+        <v>272026334041</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -3006,18 +3006,18 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="D106" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E106" t="n">
-        <v>66.67</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>272026334041</v>
+        <v>272025627677</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -3025,56 +3025,56 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1191</v>
+        <v>1199</v>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E107" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>272025627677</v>
+        <v>272025609122</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1199</v>
+        <v>1203</v>
       </c>
       <c r="D108" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E108" t="n">
-        <v>77.78</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>272025609122</v>
+        <v>272025637501</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>1203</v>
+        <v>1211</v>
       </c>
       <c r="D109" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E109" t="n">
-        <v>11.11</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>272025637501</v>
+        <v>272025627599</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -3082,18 +3082,18 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1211</v>
+        <v>1219</v>
       </c>
       <c r="D110" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E110" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>272025627599</v>
+        <v>272025616740</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -3101,18 +3101,18 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>1219</v>
+        <v>1231</v>
       </c>
       <c r="D111" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E111" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>272025616740</v>
+        <v>272026334061</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -3120,56 +3120,56 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="D112" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E112" t="n">
-        <v>88.89</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>272026334061</v>
+        <v>272025647540</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>1233</v>
+        <v>1239</v>
       </c>
       <c r="D113" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E113" t="n">
-        <v>22.22</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>272025647540</v>
+        <v>272025647543</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1239</v>
+        <v>1242</v>
       </c>
       <c r="D114" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E114" t="n">
-        <v>33.33</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>272025647543</v>
+        <v>272025660283</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -3177,56 +3177,56 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1242</v>
+        <v>1254</v>
       </c>
       <c r="D115" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E115" t="n">
-        <v>11.11</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>272025660283</v>
+        <v>272025647502</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>1254</v>
+        <v>1272</v>
       </c>
       <c r="D116" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E116" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>272025647502</v>
+        <v>272025677684</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1272</v>
+        <v>1281</v>
       </c>
       <c r="D117" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E117" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>272025677684</v>
+        <v>272025625560</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -3234,10 +3234,10 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1281</v>
+        <v>1289</v>
       </c>
       <c r="D118" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E118" t="n">
         <v>88.89</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>272025625560</v>
+        <v>272025627232</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -3253,18 +3253,18 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1289</v>
+        <v>1325</v>
       </c>
       <c r="D119" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E119" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>272025627232</v>
+        <v>272026330414</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -3272,18 +3272,18 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>1325</v>
+        <v>1334</v>
       </c>
       <c r="D120" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E120" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>272026330414</v>
+        <v>272025647376</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -3291,18 +3291,18 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1334</v>
+        <v>1336</v>
       </c>
       <c r="D121" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E121" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>272025647376</v>
+        <v>272025627450</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -3310,18 +3310,18 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1336</v>
+        <v>1339</v>
       </c>
       <c r="D122" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>272025627450</v>
+        <v>272025647365</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -3329,10 +3329,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>1339</v>
+        <v>1348</v>
       </c>
       <c r="D123" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E123" t="n">
         <v>88.89</v>
@@ -3340,45 +3340,45 @@
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>272025647365</v>
+        <v>272025663156</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>1348</v>
+        <v>1358</v>
       </c>
       <c r="D124" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E124" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>272025663156</v>
+        <v>272025609104</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1358</v>
+        <v>1377</v>
       </c>
       <c r="D125" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E125" t="n">
-        <v>0</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>272025609104</v>
+        <v>272025664392</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -3386,18 +3386,18 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>1377</v>
+        <v>1394</v>
       </c>
       <c r="D126" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E126" t="n">
-        <v>77.78</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>272025664392</v>
+        <v>272025627902</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -3405,10 +3405,10 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>1394</v>
+        <v>1418</v>
       </c>
       <c r="D127" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E127" t="n">
         <v>88.89</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>272025627902</v>
+        <v>272025668632</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -3424,18 +3424,18 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1418</v>
+        <v>1420</v>
       </c>
       <c r="D128" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E128" t="n">
-        <v>88.89</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>272025668632</v>
+        <v>272026334073</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -3443,18 +3443,18 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>1420</v>
+        <v>1423</v>
       </c>
       <c r="D129" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E129" t="n">
-        <v>55.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>272026334073</v>
+        <v>272025675558</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -3462,56 +3462,56 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>1423</v>
+        <v>1428</v>
       </c>
       <c r="D130" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E130" t="n">
-        <v>0</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>272025675558</v>
+        <v>272026330405</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1428</v>
+        <v>1430</v>
       </c>
       <c r="D131" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E131" t="n">
-        <v>77.78</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>272026330405</v>
+        <v>272025627234</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>1430</v>
+        <v>0</v>
       </c>
       <c r="D132" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E132" t="n">
-        <v>11.11</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>272025647409</v>
+        <v>272025635012</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -3519,18 +3519,18 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>1433</v>
+        <v>0</v>
       </c>
       <c r="D133" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E133" t="n">
-        <v>66.67</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>272025627234</v>
+        <v>272025641528</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -3541,15 +3541,15 @@
         <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E134" t="n">
-        <v>66.67</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>272025635012</v>
+        <v>272025666676</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -3560,15 +3560,15 @@
         <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E135" t="n">
-        <v>88.89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>272025641528</v>
+        <v>272026769336</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -3579,15 +3579,15 @@
         <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E136" t="n">
-        <v>44.44</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>272025666676</v>
+        <v>272026771781</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -3598,15 +3598,15 @@
         <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E137" t="n">
-        <v>0</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>272026769336</v>
+        <v>272027236279</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -3617,19 +3617,19 @@
         <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E138" t="n">
-        <v>66.67</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>272026771781</v>
+        <v>272027301807</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -3639,54 +3639,54 @@
         <v>3</v>
       </c>
       <c r="E139" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>272027236279</v>
+        <v>272027336447</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C140" t="n">
         <v>0</v>
       </c>
       <c r="D140" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E140" t="n">
-        <v>77.78</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>272027301807</v>
+        <v>272027443002</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C141" t="n">
         <v>0</v>
       </c>
       <c r="D141" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E141" t="n">
-        <v>0</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>272027336447</v>
+        <v>272027592893</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -3696,12 +3696,12 @@
         <v>4</v>
       </c>
       <c r="E142" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>272027443002</v>
+        <v>272027615470</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -3712,26 +3712,26 @@
         <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E143" t="n">
-        <v>33.33</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>272027592893</v>
+        <v>272027646981</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C144" t="n">
         <v>0</v>
       </c>
       <c r="D144" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E144" t="n">
         <v>0</v>
@@ -3739,26 +3739,26 @@
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>272027615470</v>
+        <v>272027764205</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C145" t="n">
         <v>0</v>
       </c>
       <c r="D145" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E145" t="n">
-        <v>11.11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>272027646981</v>
+        <v>272028072828</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>272027764205</v>
+        <v>272028559137</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -3788,7 +3788,7 @@
         <v>0</v>
       </c>
       <c r="D147" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E147" t="n">
         <v>0</v>
@@ -3796,7 +3796,7 @@
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>272028072828</v>
+        <v>272028561707</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -3807,7 +3807,7 @@
         <v>0</v>
       </c>
       <c r="D148" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E148" t="n">
         <v>0</v>
@@ -3815,26 +3815,26 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>272028559137</v>
+        <v>272028562938</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C149" t="n">
         <v>0</v>
       </c>
       <c r="D149" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E149" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>272028561707</v>
+        <v>272028605249</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -3845,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="D150" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E150" t="n">
         <v>0</v>
@@ -3853,7 +3853,7 @@
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>272028562938</v>
+        <v>272028610872</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -3864,19 +3864,19 @@
         <v>0</v>
       </c>
       <c r="D151" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E151" t="n">
-        <v>22.22</v>
+        <v>77.78</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>272028605249</v>
+        <v>272028725616</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -3886,50 +3886,50 @@
         <v>2</v>
       </c>
       <c r="E152" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>272028610872</v>
+        <v>272028873224</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C153" t="n">
         <v>0</v>
       </c>
       <c r="D153" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E153" t="n">
-        <v>77.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>272028725616</v>
+        <v>272029115693</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C154" t="n">
         <v>0</v>
       </c>
       <c r="D154" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E154" t="n">
-        <v>44.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>272028873224</v>
+        <v>272029282241</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -3940,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="D155" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E155" t="n">
         <v>0</v>
@@ -3948,7 +3948,7 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>272029115693</v>
+        <v>272029286320</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -3959,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="D156" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E156" t="n">
         <v>0</v>
@@ -3967,7 +3967,7 @@
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>272029282241</v>
+        <v>272029554204</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -3978,7 +3978,7 @@
         <v>0</v>
       </c>
       <c r="D157" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E157" t="n">
         <v>0</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>272029286320</v>
+        <v>272029669154</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -4005,11 +4005,11 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>272029554204</v>
+        <v>272029728832</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -4024,37 +4024,37 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>272029669154</v>
+        <v>272029743798</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C160" t="n">
         <v>0</v>
       </c>
       <c r="D160" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E160" t="n">
-        <v>0</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>272029728832</v>
+        <v>272029812199</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C161" t="n">
         <v>0</v>
       </c>
       <c r="D161" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E161" t="n">
         <v>0</v>
@@ -4062,7 +4062,7 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>272029743798</v>
+        <v>272029897120</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -4073,15 +4073,15 @@
         <v>0</v>
       </c>
       <c r="D162" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E162" t="n">
-        <v>44.44</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>272029812199</v>
+        <v>272030043358</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -4092,7 +4092,7 @@
         <v>0</v>
       </c>
       <c r="D163" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E163" t="n">
         <v>0</v>
@@ -4100,26 +4100,26 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>272029897120</v>
+        <v>272030065396</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C164" t="n">
         <v>0</v>
       </c>
       <c r="D164" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E164" t="n">
-        <v>66.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>272030043358</v>
+        <v>272030065415</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -4130,7 +4130,7 @@
         <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E165" t="n">
         <v>0</v>
@@ -4138,7 +4138,7 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>272030065396</v>
+        <v>272030138861</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -4149,7 +4149,7 @@
         <v>0</v>
       </c>
       <c r="D166" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E166" t="n">
         <v>0</v>
@@ -4157,18 +4157,18 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>272030065415</v>
+        <v>272030166458</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C167" t="n">
         <v>0</v>
       </c>
       <c r="D167" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E167" t="n">
         <v>0</v>
@@ -4176,26 +4176,26 @@
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>272030138861</v>
+        <v>272030201549</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C168" t="n">
         <v>0</v>
       </c>
       <c r="D168" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E168" t="n">
-        <v>0</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>272030166458</v>
+        <v>272030201552</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -4206,7 +4206,7 @@
         <v>0</v>
       </c>
       <c r="D169" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E169" t="n">
         <v>0</v>
@@ -4214,7 +4214,7 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>272030201549</v>
+        <v>272030201560</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -4225,19 +4225,19 @@
         <v>0</v>
       </c>
       <c r="D170" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E170" t="n">
-        <v>22.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>272030201552</v>
+        <v>272030211548</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -4252,7 +4252,7 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>272030201560</v>
+        <v>272030211550</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -4271,18 +4271,18 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>272030211548</v>
+        <v>272030211551</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C173" t="n">
         <v>0</v>
       </c>
       <c r="D173" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E173" t="n">
         <v>0</v>
@@ -4290,18 +4290,18 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>272030211550</v>
+        <v>272030211553</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C174" t="n">
         <v>0</v>
       </c>
       <c r="D174" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E174" t="n">
         <v>0</v>
@@ -4309,18 +4309,18 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>272030211551</v>
+        <v>272030211555</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C175" t="n">
         <v>0</v>
       </c>
       <c r="D175" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E175" t="n">
         <v>0</v>
@@ -4328,7 +4328,7 @@
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>272030211553</v>
+        <v>272030211556</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -4339,7 +4339,7 @@
         <v>0</v>
       </c>
       <c r="D176" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E176" t="n">
         <v>0</v>
@@ -4347,18 +4347,18 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>272030211555</v>
+        <v>272030211558</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Ported</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="C177" t="n">
         <v>0</v>
       </c>
       <c r="D177" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E177" t="n">
         <v>0</v>
@@ -4366,7 +4366,7 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>272030211556</v>
+        <v>272030211561</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -4385,58 +4385,20 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>272030211558</v>
+        <v>272030211563</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Ported</t>
         </is>
       </c>
       <c r="C179" t="n">
         <v>0</v>
       </c>
       <c r="D179" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E179" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="n">
-        <v>272030211561</v>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C180" t="n">
-        <v>0</v>
-      </c>
-      <c r="D180" t="n">
-        <v>3</v>
-      </c>
-      <c r="E180" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="n">
-        <v>272030211563</v>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>Ported</t>
-        </is>
-      </c>
-      <c r="C181" t="n">
-        <v>0</v>
-      </c>
-      <c r="D181" t="n">
-        <v>3</v>
-      </c>
-      <c r="E181" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>